<commit_message>
in the middle of gathering data for lab report
</commit_message>
<xml_diff>
--- a/A5/A5.xlsx
+++ b/A5/A5.xlsx
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E255"/>
+  <dimension ref="A2:I255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,7 +411,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -424,8 +424,17 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2">
+        <v>20000</v>
+      </c>
+      <c r="I2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -442,7 +451,7 @@
         <v>321.51600000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -459,12 +468,12 @@
         <v>848930.53187148587</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -477,8 +486,14 @@
       <c r="E6">
         <v>-1052</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>-1052</v>
+      </c>
+      <c r="H6">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>-1001</v>
       </c>
@@ -488,8 +503,14 @@
       <c r="E7">
         <v>-1003</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>-1001</v>
+      </c>
+      <c r="H7">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>-1060</v>
       </c>
@@ -499,8 +520,14 @@
       <c r="E8">
         <v>-1069</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>-1060</v>
+      </c>
+      <c r="H8">
+        <v>-1060</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>987</v>
       </c>
@@ -510,8 +537,14 @@
       <c r="E9">
         <v>973</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>987</v>
+      </c>
+      <c r="H9">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>976</v>
       </c>
@@ -521,8 +554,14 @@
       <c r="E10">
         <v>976</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>978</v>
+      </c>
+      <c r="H10">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>917</v>
       </c>
@@ -532,8 +571,14 @@
       <c r="E11">
         <v>-1028</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>965</v>
+      </c>
+      <c r="H11">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>968</v>
       </c>
@@ -543,8 +588,14 @@
       <c r="E12">
         <v>968</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>-1025</v>
+      </c>
+      <c r="H12">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>979</v>
       </c>
@@ -554,8 +605,14 @@
       <c r="E13">
         <v>973</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>973</v>
+      </c>
+      <c r="H13">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>994</v>
       </c>
@@ -565,8 +622,14 @@
       <c r="E14">
         <v>994</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>-1002</v>
+      </c>
+      <c r="H14">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>905</v>
       </c>
@@ -576,8 +639,14 @@
       <c r="E15">
         <v>969</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>913</v>
+      </c>
+      <c r="H15">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>-1054</v>
       </c>
@@ -587,8 +656,14 @@
       <c r="E16">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>-1001</v>
+      </c>
+      <c r="H16">
+        <v>-1054</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>978</v>
       </c>
@@ -598,8 +673,14 @@
       <c r="E17">
         <v>-1016</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>-1016</v>
+      </c>
+      <c r="H17">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>993</v>
       </c>
@@ -609,8 +690,14 @@
       <c r="E18">
         <v>989</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>993</v>
+      </c>
+      <c r="H18">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>975</v>
       </c>
@@ -620,8 +707,14 @@
       <c r="E19">
         <v>969</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>974</v>
+      </c>
+      <c r="H19">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>-1004</v>
       </c>
@@ -631,8 +724,14 @@
       <c r="E20">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>-1001</v>
+      </c>
+      <c r="H20">
+        <v>-1004</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>991</v>
       </c>
@@ -642,8 +741,14 @@
       <c r="E21">
         <v>981</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>987</v>
+      </c>
+      <c r="H21">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>964</v>
       </c>
@@ -653,8 +758,14 @@
       <c r="E22">
         <v>972</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>968</v>
+      </c>
+      <c r="H22">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>982</v>
       </c>
@@ -664,8 +775,14 @@
       <c r="E23">
         <v>984</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>-1002</v>
+      </c>
+      <c r="H23">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>965</v>
       </c>
@@ -675,8 +792,14 @@
       <c r="E24">
         <v>971</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>971</v>
+      </c>
+      <c r="H24">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>-1052</v>
       </c>
@@ -686,8 +809,14 @@
       <c r="E25">
         <v>-1052</v>
       </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>-1052</v>
+      </c>
+      <c r="H25">
+        <v>-1052</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>-1001</v>
       </c>
@@ -697,8 +826,14 @@
       <c r="E26">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>-1001</v>
+      </c>
+      <c r="H26">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>994</v>
       </c>
@@ -708,8 +843,14 @@
       <c r="E27">
         <v>988</v>
       </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>988</v>
+      </c>
+      <c r="H27">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>-1027</v>
       </c>
@@ -719,8 +860,14 @@
       <c r="E28">
         <v>-1027</v>
       </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>-1015</v>
+      </c>
+      <c r="H28">
+        <v>-1027</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>994</v>
       </c>
@@ -730,8 +877,14 @@
       <c r="E29">
         <v>994</v>
       </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>990</v>
+      </c>
+      <c r="H29">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>-99</v>
       </c>
@@ -741,8 +894,14 @@
       <c r="E30">
         <v>-99</v>
       </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>-99</v>
+      </c>
+      <c r="H30">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>-1008</v>
       </c>
@@ -752,8 +911,14 @@
       <c r="E31">
         <v>-1008</v>
       </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>-1013</v>
+      </c>
+      <c r="H31">
+        <v>-1008</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>986</v>
       </c>
@@ -763,8 +928,14 @@
       <c r="E32">
         <v>986</v>
       </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>982</v>
+      </c>
+      <c r="H32">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C33">
         <v>982</v>
       </c>
@@ -774,8 +945,14 @@
       <c r="E33">
         <v>975</v>
       </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>981</v>
+      </c>
+      <c r="H33">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C34">
         <v>923</v>
       </c>
@@ -785,8 +962,14 @@
       <c r="E34">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>-1001</v>
+      </c>
+      <c r="H34">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>994</v>
       </c>
@@ -796,8 +979,14 @@
       <c r="E35">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>-1002</v>
+      </c>
+      <c r="H35">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C36">
         <v>991</v>
       </c>
@@ -807,8 +996,14 @@
       <c r="E36">
         <v>987</v>
       </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>985</v>
+      </c>
+      <c r="H36">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C37">
         <v>-1070</v>
       </c>
@@ -818,8 +1013,14 @@
       <c r="E37">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>916</v>
+      </c>
+      <c r="H37">
+        <v>-1070</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>958</v>
       </c>
@@ -829,8 +1030,14 @@
       <c r="E38">
         <v>-50</v>
       </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>-50</v>
+      </c>
+      <c r="H38">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>968</v>
       </c>
@@ -840,8 +1047,14 @@
       <c r="E39">
         <v>968</v>
       </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>920</v>
+      </c>
+      <c r="H39">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>-1001</v>
       </c>
@@ -851,8 +1064,14 @@
       <c r="E40">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>-1001</v>
+      </c>
+      <c r="H40">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>992</v>
       </c>
@@ -862,8 +1081,14 @@
       <c r="E41">
         <v>976</v>
       </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>984</v>
+      </c>
+      <c r="H41">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>-1052</v>
       </c>
@@ -873,8 +1098,14 @@
       <c r="E42">
         <v>-1052</v>
       </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>-1052</v>
+      </c>
+      <c r="H42">
+        <v>-1052</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>980</v>
       </c>
@@ -884,8 +1115,14 @@
       <c r="E43">
         <v>982</v>
       </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>976</v>
+      </c>
+      <c r="H43">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>-1001</v>
       </c>
@@ -895,8 +1132,14 @@
       <c r="E44">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>983</v>
+      </c>
+      <c r="H44">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C45">
         <v>988</v>
       </c>
@@ -906,8 +1149,14 @@
       <c r="E45">
         <v>994</v>
       </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>994</v>
+      </c>
+      <c r="H45">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>985</v>
       </c>
@@ -917,8 +1166,14 @@
       <c r="E46">
         <v>991</v>
       </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>991</v>
+      </c>
+      <c r="H46">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C47">
         <v>986</v>
       </c>
@@ -928,8 +1183,14 @@
       <c r="E47">
         <v>991</v>
       </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>986</v>
+      </c>
+      <c r="H47">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>-99</v>
       </c>
@@ -939,8 +1200,14 @@
       <c r="E48">
         <v>-50</v>
       </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>-99</v>
+      </c>
+      <c r="H48">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C49">
         <v>957</v>
       </c>
@@ -950,8 +1217,14 @@
       <c r="E49">
         <v>930</v>
       </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>920</v>
+      </c>
+      <c r="H49">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C50">
         <v>981</v>
       </c>
@@ -961,8 +1234,14 @@
       <c r="E50">
         <v>985</v>
       </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>956</v>
+      </c>
+      <c r="H50">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C51">
         <v>981</v>
       </c>
@@ -972,8 +1251,14 @@
       <c r="E51">
         <v>983</v>
       </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>921</v>
+      </c>
+      <c r="H51">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C52">
         <v>989</v>
       </c>
@@ -983,8 +1268,14 @@
       <c r="E52">
         <v>993</v>
       </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>985</v>
+      </c>
+      <c r="H52">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C53">
         <v>-1002</v>
       </c>
@@ -994,8 +1285,14 @@
       <c r="E53">
         <v>-1060</v>
       </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>-1017</v>
+      </c>
+      <c r="H53">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C54">
         <v>939</v>
       </c>
@@ -1005,8 +1302,14 @@
       <c r="E54">
         <v>932</v>
       </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>934</v>
+      </c>
+      <c r="H54">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C55">
         <v>909</v>
       </c>
@@ -1016,8 +1319,14 @@
       <c r="E55">
         <v>913</v>
       </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>-1035</v>
+      </c>
+      <c r="H55">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C56">
         <v>983</v>
       </c>
@@ -1027,8 +1336,14 @@
       <c r="E56">
         <v>983</v>
       </c>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>977</v>
+      </c>
+      <c r="H56">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C57">
         <v>-1006</v>
       </c>
@@ -1038,8 +1353,14 @@
       <c r="E57">
         <v>-1006</v>
       </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>-1002</v>
+      </c>
+      <c r="H57">
+        <v>-1006</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C58">
         <v>993</v>
       </c>
@@ -1049,8 +1370,14 @@
       <c r="E58">
         <v>991</v>
       </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>981</v>
+      </c>
+      <c r="H58">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C59">
         <v>989</v>
       </c>
@@ -1060,8 +1387,14 @@
       <c r="E59">
         <v>989</v>
       </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>993</v>
+      </c>
+      <c r="H59">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C60">
         <v>-1002</v>
       </c>
@@ -1071,8 +1404,14 @@
       <c r="E60">
         <v>-1003</v>
       </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>-1002</v>
+      </c>
+      <c r="H60">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C61">
         <v>994</v>
       </c>
@@ -1082,8 +1421,14 @@
       <c r="E61">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>994</v>
+      </c>
+      <c r="H61">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C62">
         <v>993</v>
       </c>
@@ -1093,8 +1438,14 @@
       <c r="E62">
         <v>989</v>
       </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>993</v>
+      </c>
+      <c r="H62">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C63">
         <v>963</v>
       </c>
@@ -1104,8 +1455,14 @@
       <c r="E63">
         <v>963</v>
       </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>915</v>
+      </c>
+      <c r="H63">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C64">
         <v>-1002</v>
       </c>
@@ -1115,8 +1472,14 @@
       <c r="E64">
         <v>992</v>
       </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>-1002</v>
+      </c>
+      <c r="H64">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C65">
         <v>-1002</v>
       </c>
@@ -1126,8 +1489,14 @@
       <c r="E65">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>-1002</v>
+      </c>
+      <c r="H65">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C66">
         <v>977</v>
       </c>
@@ -1137,8 +1506,14 @@
       <c r="E66">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>-1001</v>
+      </c>
+      <c r="H66">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C67">
         <v>-1025</v>
       </c>
@@ -1148,8 +1523,14 @@
       <c r="E67">
         <v>-1081</v>
       </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>914</v>
+      </c>
+      <c r="H67">
+        <v>-1025</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C68">
         <v>989</v>
       </c>
@@ -1159,8 +1540,14 @@
       <c r="E68">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>-1001</v>
+      </c>
+      <c r="H68">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C69">
         <v>981</v>
       </c>
@@ -1170,8 +1557,14 @@
       <c r="E69">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>-1001</v>
+      </c>
+      <c r="H69">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C70">
         <v>-1001</v>
       </c>
@@ -1181,8 +1574,14 @@
       <c r="E70">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <v>993</v>
+      </c>
+      <c r="H70">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C71">
         <v>943</v>
       </c>
@@ -1192,8 +1591,14 @@
       <c r="E71">
         <v>939</v>
       </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>939</v>
+      </c>
+      <c r="H71">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C72">
         <v>990</v>
       </c>
@@ -1203,8 +1608,14 @@
       <c r="E72">
         <v>960</v>
       </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>976</v>
+      </c>
+      <c r="H72">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C73">
         <v>-1065</v>
       </c>
@@ -1214,8 +1625,14 @@
       <c r="E73">
         <v>-1073</v>
       </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>-1022</v>
+      </c>
+      <c r="H73">
+        <v>-1065</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C74">
         <v>-1007</v>
       </c>
@@ -1225,8 +1642,14 @@
       <c r="E74">
         <v>974</v>
       </c>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>-1013</v>
+      </c>
+      <c r="H74">
+        <v>-1007</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C75">
         <v>-1019</v>
       </c>
@@ -1236,8 +1659,14 @@
       <c r="E75">
         <v>-1073</v>
       </c>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>-1076</v>
+      </c>
+      <c r="H75">
+        <v>-1019</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C76">
         <v>-1014</v>
       </c>
@@ -1247,8 +1676,14 @@
       <c r="E76">
         <v>-1012</v>
       </c>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>-1013</v>
+      </c>
+      <c r="H76">
+        <v>-1014</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C77">
         <v>987</v>
       </c>
@@ -1258,8 +1693,14 @@
       <c r="E77">
         <v>913</v>
       </c>
-    </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <v>913</v>
+      </c>
+      <c r="H77">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C78">
         <v>957</v>
       </c>
@@ -1269,8 +1710,14 @@
       <c r="E78">
         <v>969</v>
       </c>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <v>975</v>
+      </c>
+      <c r="H78">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C79">
         <v>989</v>
       </c>
@@ -1280,8 +1727,14 @@
       <c r="E79">
         <v>922</v>
       </c>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <v>983</v>
+      </c>
+      <c r="H79">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C80">
         <v>982</v>
       </c>
@@ -1291,8 +1744,14 @@
       <c r="E80">
         <v>973</v>
       </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <v>970</v>
+      </c>
+      <c r="H80">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C81">
         <v>979</v>
       </c>
@@ -1302,8 +1761,14 @@
       <c r="E81">
         <v>983</v>
       </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <v>983</v>
+      </c>
+      <c r="H81">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C82">
         <v>990</v>
       </c>
@@ -1313,8 +1778,14 @@
       <c r="E82">
         <v>986</v>
       </c>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <v>991</v>
+      </c>
+      <c r="H82">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C83">
         <v>912</v>
       </c>
@@ -1324,8 +1795,14 @@
       <c r="E83">
         <v>918</v>
       </c>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <v>980</v>
+      </c>
+      <c r="H83">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C84">
         <v>968</v>
       </c>
@@ -1335,8 +1812,14 @@
       <c r="E84">
         <v>-1016</v>
       </c>
-    </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <v>964</v>
+      </c>
+      <c r="H84">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C85">
         <v>988</v>
       </c>
@@ -1346,8 +1829,14 @@
       <c r="E85">
         <v>991</v>
       </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <v>990</v>
+      </c>
+      <c r="H85">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C86">
         <v>966</v>
       </c>
@@ -1357,8 +1846,14 @@
       <c r="E86">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <v>-1002</v>
+      </c>
+      <c r="H86">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C87">
         <v>-1086</v>
       </c>
@@ -1368,8 +1863,14 @@
       <c r="E87">
         <v>-1066</v>
       </c>
-    </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <v>920</v>
+      </c>
+      <c r="H87">
+        <v>-1086</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C88">
         <v>923</v>
       </c>
@@ -1379,8 +1880,14 @@
       <c r="E88">
         <v>915</v>
       </c>
-    </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <v>915</v>
+      </c>
+      <c r="H88">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C89">
         <v>975</v>
       </c>
@@ -1390,8 +1897,14 @@
       <c r="E89">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G89">
+        <v>-1001</v>
+      </c>
+      <c r="H89">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C90">
         <v>-1007</v>
       </c>
@@ -1401,8 +1914,14 @@
       <c r="E90">
         <v>-1008</v>
       </c>
-    </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G90">
+        <v>-1013</v>
+      </c>
+      <c r="H90">
+        <v>-1007</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C91">
         <v>986</v>
       </c>
@@ -1412,8 +1931,14 @@
       <c r="E91">
         <v>974</v>
       </c>
-    </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G91">
+        <v>968</v>
+      </c>
+      <c r="H91">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C92">
         <v>-1052</v>
       </c>
@@ -1423,8 +1948,14 @@
       <c r="E92">
         <v>926</v>
       </c>
-    </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <v>-1052</v>
+      </c>
+      <c r="H92">
+        <v>-1052</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C93">
         <v>990</v>
       </c>
@@ -1434,8 +1965,14 @@
       <c r="E93">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <v>980</v>
+      </c>
+      <c r="H93">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C94">
         <v>912</v>
       </c>
@@ -1445,8 +1982,14 @@
       <c r="E94">
         <v>978</v>
       </c>
-    </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <v>974</v>
+      </c>
+      <c r="H94">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C95">
         <v>993</v>
       </c>
@@ -1456,8 +1999,14 @@
       <c r="E95">
         <v>989</v>
       </c>
-    </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <v>989</v>
+      </c>
+      <c r="H95">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C96">
         <v>967</v>
       </c>
@@ -1467,8 +2016,14 @@
       <c r="E96">
         <v>969</v>
       </c>
-    </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <v>975</v>
+      </c>
+      <c r="H96">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C97">
         <v>907</v>
       </c>
@@ -1478,8 +2033,14 @@
       <c r="E97">
         <v>913</v>
       </c>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G97">
+        <v>-1001</v>
+      </c>
+      <c r="H97">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C98">
         <v>992</v>
       </c>
@@ -1489,8 +2050,14 @@
       <c r="E98">
         <v>976</v>
       </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <v>992</v>
+      </c>
+      <c r="H98">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C99">
         <v>991</v>
       </c>
@@ -1500,8 +2067,14 @@
       <c r="E99">
         <v>990</v>
       </c>
-    </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <v>991</v>
+      </c>
+      <c r="H99">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C100">
         <v>985</v>
       </c>
@@ -1511,8 +2084,14 @@
       <c r="E100">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <v>985</v>
+      </c>
+      <c r="H100">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C101">
         <v>979</v>
       </c>
@@ -1522,8 +2101,14 @@
       <c r="E101">
         <v>971</v>
       </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <v>967</v>
+      </c>
+      <c r="H101">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C102">
         <v>975</v>
       </c>
@@ -1533,8 +2118,14 @@
       <c r="E102">
         <v>975</v>
       </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G102">
+        <v>975</v>
+      </c>
+      <c r="H102">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C103">
         <v>986</v>
       </c>
@@ -1544,8 +2135,14 @@
       <c r="E103">
         <v>990</v>
       </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G103">
+        <v>994</v>
+      </c>
+      <c r="H103">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C104">
         <v>959</v>
       </c>
@@ -1555,8 +2152,14 @@
       <c r="E104">
         <v>955</v>
       </c>
-    </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <v>961</v>
+      </c>
+      <c r="H104">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="105" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C105">
         <v>929</v>
       </c>
@@ -1566,8 +2169,14 @@
       <c r="E105">
         <v>981</v>
       </c>
-    </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G105">
+        <v>-1060</v>
+      </c>
+      <c r="H105">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C106">
         <v>953</v>
       </c>
@@ -1577,8 +2186,14 @@
       <c r="E106">
         <v>953</v>
       </c>
-    </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <v>-1036</v>
+      </c>
+      <c r="H106">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C107">
         <v>914</v>
       </c>
@@ -1588,8 +2203,14 @@
       <c r="E107">
         <v>918</v>
       </c>
-    </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G107">
+        <v>-1052</v>
+      </c>
+      <c r="H107">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C108">
         <v>-1002</v>
       </c>
@@ -1599,8 +2220,14 @@
       <c r="E108">
         <v>994</v>
       </c>
-    </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G108">
+        <v>-1002</v>
+      </c>
+      <c r="H108">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C109">
         <v>-1064</v>
       </c>
@@ -1610,8 +2237,14 @@
       <c r="E109">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G109">
+        <v>-1002</v>
+      </c>
+      <c r="H109">
+        <v>-1064</v>
+      </c>
+    </row>
+    <row r="110" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C110">
         <v>952</v>
       </c>
@@ -1621,8 +2254,14 @@
       <c r="E110">
         <v>980</v>
       </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G110">
+        <v>972</v>
+      </c>
+      <c r="H110">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C111">
         <v>-1052</v>
       </c>
@@ -1632,8 +2271,14 @@
       <c r="E111">
         <v>920</v>
       </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G111">
+        <v>-1052</v>
+      </c>
+      <c r="H111">
+        <v>-1052</v>
+      </c>
+    </row>
+    <row r="112" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C112">
         <v>-1002</v>
       </c>
@@ -1643,8 +2288,14 @@
       <c r="E112">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <v>-1002</v>
+      </c>
+      <c r="H112">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C113">
         <v>-1012</v>
       </c>
@@ -1654,8 +2305,14 @@
       <c r="E113">
         <v>-1012</v>
       </c>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G113">
+        <v>-1013</v>
+      </c>
+      <c r="H113">
+        <v>-1012</v>
+      </c>
+    </row>
+    <row r="114" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C114">
         <v>-1001</v>
       </c>
@@ -1665,8 +2322,14 @@
       <c r="E114">
         <v>953</v>
       </c>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G114">
+        <v>-1001</v>
+      </c>
+      <c r="H114">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C115">
         <v>987</v>
       </c>
@@ -1676,8 +2339,14 @@
       <c r="E115">
         <v>987</v>
       </c>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G115">
+        <v>975</v>
+      </c>
+      <c r="H115">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C116">
         <v>992</v>
       </c>
@@ -1687,8 +2356,14 @@
       <c r="E116">
         <v>992</v>
       </c>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G116">
+        <v>-1002</v>
+      </c>
+      <c r="H116">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C117">
         <v>916</v>
       </c>
@@ -1698,8 +2373,14 @@
       <c r="E117">
         <v>922</v>
       </c>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G117">
+        <v>-1052</v>
+      </c>
+      <c r="H117">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="118" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C118">
         <v>-1002</v>
       </c>
@@ -1709,8 +2390,14 @@
       <c r="E118">
         <v>984</v>
       </c>
-    </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G118">
+        <v>982</v>
+      </c>
+      <c r="H118">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="119" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C119">
         <v>977</v>
       </c>
@@ -1720,8 +2407,14 @@
       <c r="E119">
         <v>973</v>
       </c>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G119">
+        <v>981</v>
+      </c>
+      <c r="H119">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="120" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C120">
         <v>916</v>
       </c>
@@ -1731,8 +2424,14 @@
       <c r="E120">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G120">
+        <v>-1002</v>
+      </c>
+      <c r="H120">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C121">
         <v>-1078</v>
       </c>
@@ -1742,8 +2441,14 @@
       <c r="E121">
         <v>-1085</v>
       </c>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G121">
+        <v>-1001</v>
+      </c>
+      <c r="H121">
+        <v>-1078</v>
+      </c>
+    </row>
+    <row r="122" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C122">
         <v>974</v>
       </c>
@@ -1753,8 +2458,14 @@
       <c r="E122">
         <v>-1041</v>
       </c>
-    </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G122">
+        <v>994</v>
+      </c>
+      <c r="H122">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="123" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C123">
         <v>991</v>
       </c>
@@ -1764,8 +2475,14 @@
       <c r="E123">
         <v>985</v>
       </c>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G123">
+        <v>987</v>
+      </c>
+      <c r="H123">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="124" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C124">
         <v>-1002</v>
       </c>
@@ -1775,8 +2492,14 @@
       <c r="E124">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G124">
+        <v>-1002</v>
+      </c>
+      <c r="H124">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="125" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C125">
         <v>901</v>
       </c>
@@ -1786,8 +2509,14 @@
       <c r="E125">
         <v>907</v>
       </c>
-    </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G125">
+        <v>909</v>
+      </c>
+      <c r="H125">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="126" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C126">
         <v>953</v>
       </c>
@@ -1797,8 +2526,14 @@
       <c r="E126">
         <v>963</v>
       </c>
-    </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G126">
+        <v>951</v>
+      </c>
+      <c r="H126">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="127" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C127">
         <v>959</v>
       </c>
@@ -1808,8 +2543,14 @@
       <c r="E127">
         <v>977</v>
       </c>
-    </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G127">
+        <v>971</v>
+      </c>
+      <c r="H127">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="128" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C128">
         <v>978</v>
       </c>
@@ -1819,8 +2560,14 @@
       <c r="E128">
         <v>975</v>
       </c>
-    </row>
-    <row r="129" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G128">
+        <v>982</v>
+      </c>
+      <c r="H128">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C129">
         <v>988</v>
       </c>
@@ -1830,8 +2577,14 @@
       <c r="E129">
         <v>994</v>
       </c>
-    </row>
-    <row r="130" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G129">
+        <v>988</v>
+      </c>
+      <c r="H129">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="130" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C130">
         <v>-50</v>
       </c>
@@ -1841,8 +2594,14 @@
       <c r="E130">
         <v>965</v>
       </c>
-    </row>
-    <row r="131" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G130">
+        <v>967</v>
+      </c>
+      <c r="H130">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="131" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C131">
         <v>909</v>
       </c>
@@ -1852,8 +2611,14 @@
       <c r="E131">
         <v>-1088</v>
       </c>
-    </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G131">
+        <v>-1032</v>
+      </c>
+      <c r="H131">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C132">
         <v>974</v>
       </c>
@@ -1863,8 +2628,14 @@
       <c r="E132">
         <v>972</v>
       </c>
-    </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G132">
+        <v>961</v>
+      </c>
+      <c r="H132">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C133">
         <v>975</v>
       </c>
@@ -1874,8 +2645,14 @@
       <c r="E133">
         <v>973</v>
       </c>
-    </row>
-    <row r="134" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G133">
+        <v>973</v>
+      </c>
+      <c r="H133">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="134" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C134">
         <v>978</v>
       </c>
@@ -1885,8 +2662,14 @@
       <c r="E134">
         <v>980</v>
       </c>
-    </row>
-    <row r="135" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G134">
+        <v>986</v>
+      </c>
+      <c r="H134">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="135" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C135">
         <v>975</v>
       </c>
@@ -1896,8 +2679,14 @@
       <c r="E135">
         <v>979</v>
       </c>
-    </row>
-    <row r="136" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G135">
+        <v>977</v>
+      </c>
+      <c r="H135">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="136" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C136">
         <v>911</v>
       </c>
@@ -1907,8 +2696,14 @@
       <c r="E136">
         <v>907</v>
       </c>
-    </row>
-    <row r="137" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G136">
+        <v>931</v>
+      </c>
+      <c r="H136">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="137" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C137">
         <v>971</v>
       </c>
@@ -1918,8 +2713,14 @@
       <c r="E137">
         <v>964</v>
       </c>
-    </row>
-    <row r="138" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G137">
+        <v>965</v>
+      </c>
+      <c r="H137">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="138" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C138">
         <v>-1001</v>
       </c>
@@ -1929,8 +2730,14 @@
       <c r="E138">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="139" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G138">
+        <v>-1001</v>
+      </c>
+      <c r="H138">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="139" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C139">
         <v>933</v>
       </c>
@@ -1940,8 +2747,14 @@
       <c r="E139">
         <v>931</v>
       </c>
-    </row>
-    <row r="140" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G139">
+        <v>925</v>
+      </c>
+      <c r="H139">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="140" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C140">
         <v>981</v>
       </c>
@@ -1951,8 +2764,14 @@
       <c r="E140">
         <v>979</v>
       </c>
-    </row>
-    <row r="141" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G140">
+        <v>971</v>
+      </c>
+      <c r="H140">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="141" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C141">
         <v>972</v>
       </c>
@@ -1962,8 +2781,14 @@
       <c r="E141">
         <v>976</v>
       </c>
-    </row>
-    <row r="142" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G141">
+        <v>973</v>
+      </c>
+      <c r="H141">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="142" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C142">
         <v>-1052</v>
       </c>
@@ -1973,8 +2798,14 @@
       <c r="E142">
         <v>918</v>
       </c>
-    </row>
-    <row r="143" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G142">
+        <v>-1052</v>
+      </c>
+      <c r="H142">
+        <v>-1052</v>
+      </c>
+    </row>
+    <row r="143" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C143">
         <v>989</v>
       </c>
@@ -1984,8 +2815,14 @@
       <c r="E143">
         <v>973</v>
       </c>
-    </row>
-    <row r="144" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G143">
+        <v>989</v>
+      </c>
+      <c r="H143">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="144" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C144">
         <v>912</v>
       </c>
@@ -1995,8 +2832,14 @@
       <c r="E144">
         <v>914</v>
       </c>
-    </row>
-    <row r="145" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G144">
+        <v>968</v>
+      </c>
+      <c r="H144">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="145" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C145">
         <v>-1065</v>
       </c>
@@ -2006,8 +2849,14 @@
       <c r="E145">
         <v>-1065</v>
       </c>
-    </row>
-    <row r="146" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G145">
+        <v>-1065</v>
+      </c>
+      <c r="H145">
+        <v>-1065</v>
+      </c>
+    </row>
+    <row r="146" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C146">
         <v>-1002</v>
       </c>
@@ -2017,8 +2866,14 @@
       <c r="E146">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="147" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G146">
+        <v>922</v>
+      </c>
+      <c r="H146">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="147" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C147">
         <v>990</v>
       </c>
@@ -2028,8 +2883,14 @@
       <c r="E147">
         <v>990</v>
       </c>
-    </row>
-    <row r="148" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G147">
+        <v>994</v>
+      </c>
+      <c r="H147">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="148" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C148">
         <v>908</v>
       </c>
@@ -2039,8 +2900,14 @@
       <c r="E148">
         <v>-1065</v>
       </c>
-    </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G148">
+        <v>916</v>
+      </c>
+      <c r="H148">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="149" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C149">
         <v>939</v>
       </c>
@@ -2050,8 +2917,14 @@
       <c r="E149">
         <v>943</v>
       </c>
-    </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G149">
+        <v>943</v>
+      </c>
+      <c r="H149">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="150" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C150">
         <v>955</v>
       </c>
@@ -2061,8 +2934,14 @@
       <c r="E150">
         <v>965</v>
       </c>
-    </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G150">
+        <v>965</v>
+      </c>
+      <c r="H150">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="151" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C151">
         <v>992</v>
       </c>
@@ -2072,8 +2951,14 @@
       <c r="E151">
         <v>970</v>
       </c>
-    </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G151">
+        <v>960</v>
+      </c>
+      <c r="H151">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="152" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C152">
         <v>-50</v>
       </c>
@@ -2083,8 +2968,14 @@
       <c r="E152">
         <v>-50</v>
       </c>
-    </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G152">
+        <v>906</v>
+      </c>
+      <c r="H152">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="153" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C153">
         <v>988</v>
       </c>
@@ -2094,8 +2985,14 @@
       <c r="E153">
         <v>994</v>
       </c>
-    </row>
-    <row r="154" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G153">
+        <v>988</v>
+      </c>
+      <c r="H153">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="154" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C154">
         <v>-1066</v>
       </c>
@@ -2105,8 +3002,14 @@
       <c r="E154">
         <v>-1073</v>
       </c>
-    </row>
-    <row r="155" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G154">
+        <v>-1065</v>
+      </c>
+      <c r="H154">
+        <v>-1066</v>
+      </c>
+    </row>
+    <row r="155" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C155">
         <v>982</v>
       </c>
@@ -2116,8 +3019,14 @@
       <c r="E155">
         <v>982</v>
       </c>
-    </row>
-    <row r="156" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G155">
+        <v>986</v>
+      </c>
+      <c r="H155">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="156" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C156">
         <v>967</v>
       </c>
@@ -2127,8 +3036,14 @@
       <c r="E156">
         <v>973</v>
       </c>
-    </row>
-    <row r="157" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G156">
+        <v>974</v>
+      </c>
+      <c r="H156">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="157" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C157">
         <v>971</v>
       </c>
@@ -2138,8 +3053,14 @@
       <c r="E157">
         <v>957</v>
       </c>
-    </row>
-    <row r="158" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G157">
+        <v>912</v>
+      </c>
+      <c r="H157">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="158" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C158">
         <v>-1064</v>
       </c>
@@ -2149,8 +3070,14 @@
       <c r="E158">
         <v>-1076</v>
       </c>
-    </row>
-    <row r="159" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G158">
+        <v>-1076</v>
+      </c>
+      <c r="H158">
+        <v>-1064</v>
+      </c>
+    </row>
+    <row r="159" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C159">
         <v>981</v>
       </c>
@@ -2160,8 +3087,14 @@
       <c r="E159">
         <v>981</v>
       </c>
-    </row>
-    <row r="160" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G159">
+        <v>977</v>
+      </c>
+      <c r="H159">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="160" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C160">
         <v>994</v>
       </c>
@@ -2171,8 +3104,14 @@
       <c r="E160">
         <v>994</v>
       </c>
-    </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G160">
+        <v>994</v>
+      </c>
+      <c r="H160">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="161" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C161">
         <v>981</v>
       </c>
@@ -2182,8 +3121,14 @@
       <c r="E161">
         <v>-1012</v>
       </c>
-    </row>
-    <row r="162" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G161">
+        <v>-1008</v>
+      </c>
+      <c r="H161">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="162" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C162">
         <v>-1002</v>
       </c>
@@ -2193,8 +3138,14 @@
       <c r="E162">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="163" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G162">
+        <v>-1002</v>
+      </c>
+      <c r="H162">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="163" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C163">
         <v>-1001</v>
       </c>
@@ -2204,8 +3155,14 @@
       <c r="E163">
         <v>991</v>
       </c>
-    </row>
-    <row r="164" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G163">
+        <v>-1004</v>
+      </c>
+      <c r="H163">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="164" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C164">
         <v>917</v>
       </c>
@@ -2215,8 +3172,14 @@
       <c r="E164">
         <v>917</v>
       </c>
-    </row>
-    <row r="165" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G164">
+        <v>911</v>
+      </c>
+      <c r="H164">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="165" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C165">
         <v>-1001</v>
       </c>
@@ -2226,8 +3189,14 @@
       <c r="E165">
         <v>-1003</v>
       </c>
-    </row>
-    <row r="166" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G165">
+        <v>-1003</v>
+      </c>
+      <c r="H165">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="166" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C166">
         <v>974</v>
       </c>
@@ -2237,8 +3206,14 @@
       <c r="E166">
         <v>980</v>
       </c>
-    </row>
-    <row r="167" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G166">
+        <v>986</v>
+      </c>
+      <c r="H166">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="167" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C167">
         <v>-1071</v>
       </c>
@@ -2248,8 +3223,14 @@
       <c r="E167">
         <v>912</v>
       </c>
-    </row>
-    <row r="168" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G167">
+        <v>-1083</v>
+      </c>
+      <c r="H167">
+        <v>-1071</v>
+      </c>
+    </row>
+    <row r="168" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C168">
         <v>983</v>
       </c>
@@ -2259,8 +3240,14 @@
       <c r="E168">
         <v>983</v>
       </c>
-    </row>
-    <row r="169" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G168">
+        <v>987</v>
+      </c>
+      <c r="H168">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="169" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C169">
         <v>990</v>
       </c>
@@ -2270,8 +3257,14 @@
       <c r="E169">
         <v>984</v>
       </c>
-    </row>
-    <row r="170" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G169">
+        <v>976</v>
+      </c>
+      <c r="H169">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="170" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C170">
         <v>953</v>
       </c>
@@ -2281,8 +3274,14 @@
       <c r="E170">
         <v>963</v>
       </c>
-    </row>
-    <row r="171" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G170">
+        <v>955</v>
+      </c>
+      <c r="H170">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="171" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C171">
         <v>-1002</v>
       </c>
@@ -2292,8 +3291,14 @@
       <c r="E171">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="172" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G171">
+        <v>-1002</v>
+      </c>
+      <c r="H171">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="172" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C172">
         <v>988</v>
       </c>
@@ -2303,8 +3308,14 @@
       <c r="E172">
         <v>988</v>
       </c>
-    </row>
-    <row r="173" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G172">
+        <v>994</v>
+      </c>
+      <c r="H172">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="173" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C173">
         <v>985</v>
       </c>
@@ -2314,8 +3325,14 @@
       <c r="E173">
         <v>987</v>
       </c>
-    </row>
-    <row r="174" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G173">
+        <v>968</v>
+      </c>
+      <c r="H173">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="174" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C174">
         <v>-1007</v>
       </c>
@@ -2325,8 +3342,14 @@
       <c r="E174">
         <v>-1007</v>
       </c>
-    </row>
-    <row r="175" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G174">
+        <v>-1013</v>
+      </c>
+      <c r="H174">
+        <v>-1007</v>
+      </c>
+    </row>
+    <row r="175" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C175">
         <v>-1015</v>
       </c>
@@ -2336,8 +3359,14 @@
       <c r="E175">
         <v>-1088</v>
       </c>
-    </row>
-    <row r="176" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G175">
+        <v>-1099</v>
+      </c>
+      <c r="H175">
+        <v>-1015</v>
+      </c>
+    </row>
+    <row r="176" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C176">
         <v>-1064</v>
       </c>
@@ -2347,8 +3376,14 @@
       <c r="E176">
         <v>-1069</v>
       </c>
-    </row>
-    <row r="177" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G176">
+        <v>-1073</v>
+      </c>
+      <c r="H176">
+        <v>-1064</v>
+      </c>
+    </row>
+    <row r="177" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C177">
         <v>-1002</v>
       </c>
@@ -2358,8 +3393,14 @@
       <c r="E177">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="178" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G177">
+        <v>942</v>
+      </c>
+      <c r="H177">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="178" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C178">
         <v>989</v>
       </c>
@@ -2369,8 +3410,14 @@
       <c r="E178">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="179" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G178">
+        <v>-1001</v>
+      </c>
+      <c r="H178">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="179" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C179">
         <v>978</v>
       </c>
@@ -2380,8 +3427,14 @@
       <c r="E179">
         <v>984</v>
       </c>
-    </row>
-    <row r="180" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G179">
+        <v>984</v>
+      </c>
+      <c r="H179">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="180" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C180">
         <v>912</v>
       </c>
@@ -2391,8 +3444,14 @@
       <c r="E180">
         <v>925</v>
       </c>
-    </row>
-    <row r="181" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G180">
+        <v>927</v>
+      </c>
+      <c r="H180">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="181" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C181">
         <v>972</v>
       </c>
@@ -2402,8 +3461,14 @@
       <c r="E181">
         <v>980</v>
       </c>
-    </row>
-    <row r="182" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G181">
+        <v>972</v>
+      </c>
+      <c r="H181">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="182" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C182">
         <v>975</v>
       </c>
@@ -2413,8 +3478,14 @@
       <c r="E182">
         <v>969</v>
       </c>
-    </row>
-    <row r="183" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G182">
+        <v>975</v>
+      </c>
+      <c r="H182">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="183" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C183">
         <v>-1069</v>
       </c>
@@ -2424,8 +3495,14 @@
       <c r="E183">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="184" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G183">
+        <v>-1002</v>
+      </c>
+      <c r="H183">
+        <v>-1069</v>
+      </c>
+    </row>
+    <row r="184" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C184">
         <v>-1001</v>
       </c>
@@ -2435,8 +3512,14 @@
       <c r="E184">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="185" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G184">
+        <v>-1007</v>
+      </c>
+      <c r="H184">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="185" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C185">
         <v>991</v>
       </c>
@@ -2446,8 +3529,14 @@
       <c r="E185">
         <v>990</v>
       </c>
-    </row>
-    <row r="186" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G185">
+        <v>988</v>
+      </c>
+      <c r="H185">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="186" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C186">
         <v>921</v>
       </c>
@@ -2457,8 +3546,14 @@
       <c r="E186">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="187" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G186">
+        <v>-1001</v>
+      </c>
+      <c r="H186">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="187" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C187">
         <v>-1002</v>
       </c>
@@ -2468,8 +3563,14 @@
       <c r="E187">
         <v>-1006</v>
       </c>
-    </row>
-    <row r="188" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G187">
+        <v>-1002</v>
+      </c>
+      <c r="H187">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="188" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C188">
         <v>985</v>
       </c>
@@ -2479,8 +3580,14 @@
       <c r="E188">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="189" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G188">
+        <v>-1001</v>
+      </c>
+      <c r="H188">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="189" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C189">
         <v>-1002</v>
       </c>
@@ -2490,8 +3597,14 @@
       <c r="E189">
         <v>990</v>
       </c>
-    </row>
-    <row r="190" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G189">
+        <v>-1002</v>
+      </c>
+      <c r="H189">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="190" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C190">
         <v>959</v>
       </c>
@@ -2501,8 +3614,14 @@
       <c r="E190">
         <v>978</v>
       </c>
-    </row>
-    <row r="191" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G190">
+        <v>988</v>
+      </c>
+      <c r="H190">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="191" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C191">
         <v>-1002</v>
       </c>
@@ -2512,8 +3631,14 @@
       <c r="E191">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="192" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G191">
+        <v>-1002</v>
+      </c>
+      <c r="H191">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="192" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C192">
         <v>991</v>
       </c>
@@ -2523,8 +3648,14 @@
       <c r="E192">
         <v>991</v>
       </c>
-    </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G192">
+        <v>955</v>
+      </c>
+      <c r="H192">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="193" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C193">
         <v>-1002</v>
       </c>
@@ -2534,8 +3665,14 @@
       <c r="E193">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="194" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G193">
+        <v>912</v>
+      </c>
+      <c r="H193">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="194" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C194">
         <v>960</v>
       </c>
@@ -2545,8 +3682,14 @@
       <c r="E194">
         <v>-50</v>
       </c>
-    </row>
-    <row r="195" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G194">
+        <v>903</v>
+      </c>
+      <c r="H194">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="195" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C195">
         <v>966</v>
       </c>
@@ -2556,8 +3699,14 @@
       <c r="E195">
         <v>958</v>
       </c>
-    </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G195">
+        <v>906</v>
+      </c>
+      <c r="H195">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="196" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C196">
         <v>901</v>
       </c>
@@ -2567,8 +3716,14 @@
       <c r="E196">
         <v>959</v>
       </c>
-    </row>
-    <row r="197" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G196">
+        <v>953</v>
+      </c>
+      <c r="H196">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="197" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C197">
         <v>971</v>
       </c>
@@ -2578,8 +3733,14 @@
       <c r="E197">
         <v>973</v>
       </c>
-    </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G197">
+        <v>973</v>
+      </c>
+      <c r="H197">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="198" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C198">
         <v>-1013</v>
       </c>
@@ -2589,8 +3750,14 @@
       <c r="E198">
         <v>926</v>
       </c>
-    </row>
-    <row r="199" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G198">
+        <v>960</v>
+      </c>
+      <c r="H198">
+        <v>-1013</v>
+      </c>
+    </row>
+    <row r="199" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C199">
         <v>-99</v>
       </c>
@@ -2600,8 +3767,14 @@
       <c r="E199">
         <v>-99</v>
       </c>
-    </row>
-    <row r="200" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G199">
+        <v>964</v>
+      </c>
+      <c r="H199">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="200" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C200">
         <v>975</v>
       </c>
@@ -2611,8 +3784,14 @@
       <c r="E200">
         <v>983</v>
       </c>
-    </row>
-    <row r="201" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G200">
+        <v>973</v>
+      </c>
+      <c r="H200">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="201" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C201">
         <v>984</v>
       </c>
@@ -2622,8 +3801,14 @@
       <c r="E201">
         <v>992</v>
       </c>
-    </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G201">
+        <v>992</v>
+      </c>
+      <c r="H201">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="202" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C202">
         <v>911</v>
       </c>
@@ -2633,8 +3818,14 @@
       <c r="E202">
         <v>901</v>
       </c>
-    </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G202">
+        <v>909</v>
+      </c>
+      <c r="H202">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="203" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C203">
         <v>991</v>
       </c>
@@ -2644,8 +3835,14 @@
       <c r="E203">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G203">
+        <v>-1001</v>
+      </c>
+      <c r="H203">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="204" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C204">
         <v>-1001</v>
       </c>
@@ -2655,8 +3852,14 @@
       <c r="E204">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G204">
+        <v>-1001</v>
+      </c>
+      <c r="H204">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="205" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C205">
         <v>954</v>
       </c>
@@ -2666,8 +3869,14 @@
       <c r="E205">
         <v>962</v>
       </c>
-    </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G205">
+        <v>968</v>
+      </c>
+      <c r="H205">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="206" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C206">
         <v>973</v>
       </c>
@@ -2677,8 +3886,14 @@
       <c r="E206">
         <v>911</v>
       </c>
-    </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G206">
+        <v>911</v>
+      </c>
+      <c r="H206">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="207" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C207">
         <v>-1079</v>
       </c>
@@ -2688,8 +3903,14 @@
       <c r="E207">
         <v>-1072</v>
       </c>
-    </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G207">
+        <v>-1077</v>
+      </c>
+      <c r="H207">
+        <v>-1079</v>
+      </c>
+    </row>
+    <row r="208" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C208">
         <v>937</v>
       </c>
@@ -2699,8 +3920,14 @@
       <c r="E208">
         <v>919</v>
       </c>
-    </row>
-    <row r="209" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G208">
+        <v>943</v>
+      </c>
+      <c r="H208">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="209" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C209">
         <v>974</v>
       </c>
@@ -2710,8 +3937,14 @@
       <c r="E209">
         <v>981</v>
       </c>
-    </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G209">
+        <v>983</v>
+      </c>
+      <c r="H209">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="210" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C210">
         <v>-1001</v>
       </c>
@@ -2721,8 +3954,14 @@
       <c r="E210">
         <v>973</v>
       </c>
-    </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G210">
+        <v>-1001</v>
+      </c>
+      <c r="H210">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="211" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C211">
         <v>-1074</v>
       </c>
@@ -2732,8 +3971,14 @@
       <c r="E211">
         <v>-1072</v>
       </c>
-    </row>
-    <row r="212" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G211">
+        <v>-1060</v>
+      </c>
+      <c r="H211">
+        <v>-1074</v>
+      </c>
+    </row>
+    <row r="212" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C212">
         <v>991</v>
       </c>
@@ -2743,8 +3988,14 @@
       <c r="E212">
         <v>990</v>
       </c>
-    </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G212">
+        <v>991</v>
+      </c>
+      <c r="H212">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="213" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C213">
         <v>990</v>
       </c>
@@ -2754,8 +4005,14 @@
       <c r="E213">
         <v>991</v>
       </c>
-    </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G213">
+        <v>986</v>
+      </c>
+      <c r="H213">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="214" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C214">
         <v>926</v>
       </c>
@@ -2765,8 +4022,14 @@
       <c r="E214">
         <v>920</v>
       </c>
-    </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G214">
+        <v>920</v>
+      </c>
+      <c r="H214">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="215" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C215">
         <v>975</v>
       </c>
@@ -2776,8 +4039,14 @@
       <c r="E215">
         <v>977</v>
       </c>
-    </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G215">
+        <v>975</v>
+      </c>
+      <c r="H215">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="216" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C216">
         <v>961</v>
       </c>
@@ -2787,8 +4056,14 @@
       <c r="E216">
         <v>917</v>
       </c>
-    </row>
-    <row r="217" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G216">
+        <v>969</v>
+      </c>
+      <c r="H216">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="217" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C217">
         <v>993</v>
       </c>
@@ -2798,8 +4073,14 @@
       <c r="E217">
         <v>-1001</v>
       </c>
-    </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G217">
+        <v>993</v>
+      </c>
+      <c r="H217">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="218" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C218">
         <v>-1006</v>
       </c>
@@ -2809,8 +4090,14 @@
       <c r="E218">
         <v>-1002</v>
       </c>
-    </row>
-    <row r="219" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G218">
+        <v>-1003</v>
+      </c>
+      <c r="H218">
+        <v>-1006</v>
+      </c>
+    </row>
+    <row r="219" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C219">
         <v>-1002</v>
       </c>
@@ -2820,8 +4107,14 @@
       <c r="E219">
         <v>976</v>
       </c>
-    </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G219">
+        <v>916</v>
+      </c>
+      <c r="H219">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="220" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C220">
         <v>977</v>
       </c>
@@ -2831,8 +4124,14 @@
       <c r="E220">
         <v>979</v>
       </c>
-    </row>
-    <row r="221" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G220">
+        <v>977</v>
+      </c>
+      <c r="H220">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="221" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C221">
         <v>-1065</v>
       </c>
@@ -2842,8 +4141,14 @@
       <c r="E221">
         <v>-1073</v>
       </c>
-    </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G221">
+        <v>-1063</v>
+      </c>
+      <c r="H221">
+        <v>-1065</v>
+      </c>
+    </row>
+    <row r="222" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C222">
         <v>988</v>
       </c>
@@ -2853,8 +4158,14 @@
       <c r="E222">
         <v>994</v>
       </c>
-    </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G222">
+        <v>994</v>
+      </c>
+      <c r="H222">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="223" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C223">
         <v>909</v>
       </c>
@@ -2864,8 +4175,14 @@
       <c r="E223">
         <v>905</v>
       </c>
-    </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G223">
+        <v>911</v>
+      </c>
+      <c r="H223">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="224" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C224">
         <v>905</v>
       </c>
@@ -2875,8 +4192,14 @@
       <c r="E224">
         <v>907</v>
       </c>
-    </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G224">
+        <v>903</v>
+      </c>
+      <c r="H224">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="225" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C225">
         <v>993</v>
       </c>
@@ -2886,8 +4209,14 @@
       <c r="E225">
         <v>989</v>
       </c>
-    </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G225">
+        <v>993</v>
+      </c>
+      <c r="H225">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="226" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C226">
         <v>993</v>
       </c>
@@ -2897,8 +4226,14 @@
       <c r="E226">
         <v>993</v>
       </c>
-    </row>
-    <row r="227" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G226">
+        <v>991</v>
+      </c>
+      <c r="H226">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="227" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C227">
         <v>-1002</v>
       </c>
@@ -2908,8 +4243,14 @@
       <c r="E227">
         <v>920</v>
       </c>
-    </row>
-    <row r="228" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G227">
+        <v>912</v>
+      </c>
+      <c r="H227">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="228" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C228">
         <v>-1001</v>
       </c>
@@ -2919,8 +4260,14 @@
       <c r="E228">
         <v>985</v>
       </c>
-    </row>
-    <row r="229" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G228">
+        <v>985</v>
+      </c>
+      <c r="H228">
+        <v>-1001</v>
+      </c>
+    </row>
+    <row r="229" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C229">
         <v>991</v>
       </c>
@@ -2930,8 +4277,14 @@
       <c r="E229">
         <v>993</v>
       </c>
-    </row>
-    <row r="230" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G229">
+        <v>971</v>
+      </c>
+      <c r="H229">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="230" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C230">
         <v>989</v>
       </c>
@@ -2941,8 +4294,14 @@
       <c r="E230">
         <v>993</v>
       </c>
-    </row>
-    <row r="231" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G230">
+        <v>989</v>
+      </c>
+      <c r="H230">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="231" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C231">
         <v>993</v>
       </c>
@@ -2952,8 +4311,14 @@
       <c r="E231">
         <v>993</v>
       </c>
-    </row>
-    <row r="232" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G231">
+        <v>991</v>
+      </c>
+      <c r="H231">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="232" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C232">
         <v>991</v>
       </c>
@@ -2963,8 +4328,14 @@
       <c r="E232">
         <v>993</v>
       </c>
-    </row>
-    <row r="233" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G232">
+        <v>987</v>
+      </c>
+      <c r="H232">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="233" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C233">
         <v>983</v>
       </c>
@@ -2974,8 +4345,14 @@
       <c r="E233">
         <v>983</v>
       </c>
-    </row>
-    <row r="234" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G233">
+        <v>983</v>
+      </c>
+      <c r="H233">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="234" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C234">
         <v>955</v>
       </c>
@@ -2985,8 +4362,14 @@
       <c r="E234">
         <v>971</v>
       </c>
-    </row>
-    <row r="235" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G234">
+        <v>969</v>
+      </c>
+      <c r="H234">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="235" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C235">
         <v>979</v>
       </c>
@@ -2996,8 +4379,14 @@
       <c r="E235">
         <v>983</v>
       </c>
-    </row>
-    <row r="236" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G235">
+        <v>977</v>
+      </c>
+      <c r="H235">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="236" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C236">
         <v>979</v>
       </c>
@@ -3007,8 +4396,14 @@
       <c r="E236">
         <v>976</v>
       </c>
-    </row>
-    <row r="237" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G236">
+        <v>977</v>
+      </c>
+      <c r="H236">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="237" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C237">
         <v>-1002</v>
       </c>
@@ -3018,8 +4413,14 @@
       <c r="E237">
         <v>-1006</v>
       </c>
-    </row>
-    <row r="238" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G237">
+        <v>-1002</v>
+      </c>
+      <c r="H237">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="238" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C238">
         <v>-1002</v>
       </c>
@@ -3029,8 +4430,14 @@
       <c r="E238">
         <v>992</v>
       </c>
-    </row>
-    <row r="239" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G238">
+        <v>992</v>
+      </c>
+      <c r="H238">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="239" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C239">
         <v>982</v>
       </c>
@@ -3040,8 +4447,14 @@
       <c r="E239">
         <v>974</v>
       </c>
-    </row>
-    <row r="240" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G239">
+        <v>986</v>
+      </c>
+      <c r="H239">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="240" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C240">
         <v>991</v>
       </c>
@@ -3051,8 +4464,14 @@
       <c r="E240">
         <v>981</v>
       </c>
-    </row>
-    <row r="241" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G240">
+        <v>981</v>
+      </c>
+      <c r="H240">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="241" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C241">
         <v>-1077</v>
       </c>
@@ -3062,8 +4481,14 @@
       <c r="E241">
         <v>-1075</v>
       </c>
-    </row>
-    <row r="242" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G241">
+        <v>-1071</v>
+      </c>
+      <c r="H241">
+        <v>-1077</v>
+      </c>
+    </row>
+    <row r="242" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C242">
         <v>981</v>
       </c>
@@ -3073,8 +4498,14 @@
       <c r="E242">
         <v>983</v>
       </c>
-    </row>
-    <row r="243" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G242">
+        <v>989</v>
+      </c>
+      <c r="H242">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="243" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C243">
         <v>-1066</v>
       </c>
@@ -3084,8 +4515,14 @@
       <c r="E243">
         <v>-1056</v>
       </c>
-    </row>
-    <row r="244" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G243">
+        <v>-1057</v>
+      </c>
+      <c r="H243">
+        <v>-1066</v>
+      </c>
+    </row>
+    <row r="244" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C244">
         <v>977</v>
       </c>
@@ -3095,8 +4532,14 @@
       <c r="E244">
         <v>975</v>
       </c>
-    </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G244">
+        <v>975</v>
+      </c>
+      <c r="H244">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="245" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C245">
         <v>984</v>
       </c>
@@ -3106,8 +4549,14 @@
       <c r="E245">
         <v>982</v>
       </c>
-    </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G245">
+        <v>976</v>
+      </c>
+      <c r="H245">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="246" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C246">
         <v>-1004</v>
       </c>
@@ -3117,8 +4566,14 @@
       <c r="E246">
         <v>-1004</v>
       </c>
-    </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G246">
+        <v>-1007</v>
+      </c>
+      <c r="H246">
+        <v>-1004</v>
+      </c>
+    </row>
+    <row r="247" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C247">
         <v>981</v>
       </c>
@@ -3128,8 +4583,14 @@
       <c r="E247">
         <v>983</v>
       </c>
-    </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G247">
+        <v>977</v>
+      </c>
+      <c r="H247">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="248" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C248">
         <v>962</v>
       </c>
@@ -3139,8 +4600,14 @@
       <c r="E248">
         <v>968</v>
       </c>
-    </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G248">
+        <v>964</v>
+      </c>
+      <c r="H248">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="249" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C249">
         <v>970</v>
       </c>
@@ -3150,8 +4617,14 @@
       <c r="E249">
         <v>962</v>
       </c>
-    </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G249">
+        <v>966</v>
+      </c>
+      <c r="H249">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="250" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C250">
         <v>981</v>
       </c>
@@ -3161,8 +4634,14 @@
       <c r="E250">
         <v>983</v>
       </c>
-    </row>
-    <row r="251" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G250">
+        <v>975</v>
+      </c>
+      <c r="H250">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="251" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C251">
         <v>972</v>
       </c>
@@ -3172,8 +4651,14 @@
       <c r="E251">
         <v>976</v>
       </c>
-    </row>
-    <row r="252" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G251">
+        <v>980</v>
+      </c>
+      <c r="H251">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="252" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C252">
         <v>918</v>
       </c>
@@ -3183,8 +4668,14 @@
       <c r="E252">
         <v>910</v>
       </c>
-    </row>
-    <row r="253" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G252">
+        <v>910</v>
+      </c>
+      <c r="H252">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="253" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C253">
         <v>978</v>
       </c>
@@ -3194,8 +4685,14 @@
       <c r="E253">
         <v>968</v>
       </c>
-    </row>
-    <row r="254" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G253">
+        <v>986</v>
+      </c>
+      <c r="H253">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="254" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C254">
         <v>911</v>
       </c>
@@ -3205,8 +4702,14 @@
       <c r="E254">
         <v>911</v>
       </c>
-    </row>
-    <row r="255" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G254">
+        <v>-99</v>
+      </c>
+      <c r="H254">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="255" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C255">
         <v>969</v>
       </c>
@@ -3215,6 +4718,12 @@
       </c>
       <c r="E255">
         <v>979</v>
+      </c>
+      <c r="G255">
+        <v>979</v>
+      </c>
+      <c r="H255">
+        <v>969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>